<commit_message>
Solved story bug,cuesheet tab and autocomplete off in all application
</commit_message>
<xml_diff>
--- a/RightsUMusicHub.UI_Prod/src/assets/template/CuesheetImport.xlsx
+++ b/RightsUMusicHub.UI_Prod/src/assets/template/CuesheetImport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="12195"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="CueSheet" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SrNo</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Movie/Album</t>
   </si>
   <si>
-    <t>Song Type</t>
+    <t>Usage Type</t>
   </si>
   <si>
     <t>TC IN</t>
@@ -61,9 +61,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -87,7 +87,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,16 +110,48 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,6 +163,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -127,14 +188,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,30 +210,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,66 +232,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,13 +265,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,37 +391,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,127 +439,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,13 +474,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,21 +509,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -571,153 +560,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -742,12 +742,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1125,8 +1125,8 @@
   <sheetPr/>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E$1:E$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
upload functionality in cuesheet
</commit_message>
<xml_diff>
--- a/RightsUMusicHub.UI_Prod/src/assets/template/CuesheetImport.xlsx
+++ b/RightsUMusicHub.UI_Prod/src/assets/template/CuesheetImport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="12195"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="CueSheet" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SrNo</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Movie/Album</t>
   </si>
   <si>
-    <t>Song Type</t>
+    <t>Usage Type</t>
   </si>
   <si>
     <t>TC IN</t>
@@ -54,16 +54,19 @@
   <si>
     <t>Duration Frame</t>
   </si>
+  <si>
+    <t>Simmba Theme 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -85,28 +88,6 @@
       <color indexed="9"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -117,6 +98,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -125,8 +135,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -134,48 +175,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,16 +189,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,20 +219,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -233,6 +229,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,31 +268,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,151 +436,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,10 +479,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -489,6 +490,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -539,15 +551,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -576,148 +579,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -742,12 +745,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1123,13 +1126,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E$1:E$1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="24.8571428571429" style="1" customWidth="1"/>
@@ -1183,6 +1186,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>